<commit_message>
FEAT: Project can output PDFs
</commit_message>
<xml_diff>
--- a/TestData/xlsx/Alumnos.xlsx
+++ b/TestData/xlsx/Alumnos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>González</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>Mariana</t>
-  </si>
-  <si>
-    <t>Gutiérrez</t>
-  </si>
-  <si>
-    <t>Vilchis</t>
-  </si>
-  <si>
-    <t>Estban</t>
   </si>
 </sst>
 </file>
@@ -389,13 +380,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
@@ -446,23 +444,6 @@
       </c>
       <c r="E3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>44444</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>